<commit_message>
more changes to fix yolk issue
</commit_message>
<xml_diff>
--- a/data/template.xlsx
+++ b/data/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinegoode/Desktop/carp-rf/shiny-app/app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinegoode/Desktop/icrf/WhoseEgg/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0DB99F-F15A-904B-9D13-2BB192A981E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5894164D-77F4-8046-84BA-EA791BC9710E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="17240" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -52,12 +52,6 @@
     <t>Membrane_SD</t>
   </si>
   <si>
-    <t>Yolk_Ave</t>
-  </si>
-  <si>
-    <t>Yolk_SD</t>
-  </si>
-  <si>
     <t>Larval_Length</t>
   </si>
   <si>
@@ -68,6 +62,12 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>Embryo_Ave</t>
+  </si>
+  <si>
+    <t>Embryo_SD</t>
   </si>
 </sst>
 </file>
@@ -910,9 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -924,13 +922,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -960,20 +958,20 @@
         <v>9</v>
       </c>
       <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
         <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="32">
     <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Warning" error="Conductivity entered falls outside of the range of the data using to train the model (274 to 781 microS/cm). The model will be forced to extrapolate when making a prediction. Would you like to proceed?" promptTitle="Water Conductivity" prompt="microS/cm" sqref="F2:F1048576" xr:uid="{7CF36FE9-74C6-8446-B40E-2C174BEF381D}">
       <formula1>274</formula1>
-      <formula2>718</formula2>
+      <formula2>781</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Error" error="Egg_Stage must be one of the following levels: 1, 2, 3, 4, 5, 6, 7, 9, BROKEN, D" promptTitle="Egg Development Stage" prompt="1, 2, 3, 4, 5, 6, 7, 8, BROKEN, or D" sqref="I2:I1048576" xr:uid="{C1000E4C-B20E-5B40-BC45-FE810291993F}">
       <formula1>"1, 2, 3, 4, 5, 6, 7, 8, BROKEN, D"</formula1>
@@ -1002,7 +1000,7 @@
       <formula1>"Y, N"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Egg Identification" prompt="Any format acceptable" sqref="A2:A1048576" xr:uid="{4B7E24F8-60B5-EF42-8742-5023933216AB}"/>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Warning" error="Yolk_Ave entered falls outside of the range of the data using to train the model (0.434 to 4.371 mm). The model will be forced to extrapolate when making a prediction. Would you like to proceed?" promptTitle="Average Yolk Diameter" prompt="mm" sqref="N2:N1048576" xr:uid="{0776C39D-DB64-AD46-AAD5-8BC1DD7441A6}">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Warning" error="Embryo_Ave entered falls outside of the range of the data using to train the model (0.434 to 4.371 mm). The model will be forced to extrapolate when making a prediction. Would you like to proceed?" promptTitle="Average Yolk Diameter" prompt="mm" sqref="N2:N1048576" xr:uid="{0776C39D-DB64-AD46-AAD5-8BC1DD7441A6}">
       <formula1>0.434</formula1>
       <formula2>4.371</formula2>
     </dataValidation>
@@ -1021,7 +1019,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Required variable names cannot be adjusted" promptTitle="Month" prompt="1 to 12" sqref="C1" xr:uid="{FDBAA811-F673-854A-80C9-3D7A48E037BA}">
       <formula1>"Month"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Warning" error="Yolk_SD entered falls outside of the range of the data using to train the model (0.005 to 1.377 mm). The model will be forced to extrapolate when making a prediction. Would you like to proceed?" promptTitle="SD of Yolk Diameter" prompt="mm" sqref="O2:O1048576" xr:uid="{D73F7FCA-DF77-0E40-8806-426B6B1AAE1F}">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Warning" error="Embryo_SD entered falls outside of the range of the data using to train the model (0.005 to 1.377 mm). The model will be forced to extrapolate when making a prediction. Would you like to proceed?" promptTitle="SD of Yolk Diameter" prompt="mm" sqref="O2:O1048576" xr:uid="{D73F7FCA-DF77-0E40-8806-426B6B1AAE1F}">
       <formula1>0.005</formula1>
       <formula2>1.377</formula2>
     </dataValidation>
@@ -1032,9 +1030,9 @@
       <formula1>1000</formula1>
       <formula2>9999</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Entry Error" error="Month must be entered as a whole number ranging from 1 to 12." promptTitle="Month" prompt="1 to 12" sqref="C2:C1048576" xr:uid="{5324F153-32C8-204B-8021-8CC2C8CF48A1}">
-      <formula1>1</formula1>
-      <formula2>12</formula2>
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Entry Error" error="Month entered falls outside of the range of the data using to train the models (4,5,6,7,8). The model will be forced to extrapolate when making a prediction. Would you like to proceed?" promptTitle="Month" prompt="1 to 12" sqref="C2:C1048576" xr:uid="{5324F153-32C8-204B-8021-8CC2C8CF48A1}">
+      <formula1>4</formula1>
+      <formula2>8</formula2>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Required variable names cannot be adjusted" promptTitle="Day of Collection" prompt="1 to 31_x000a__x000a_Self check: make sure the day falls within the range of days for the corresponding month" sqref="D1" xr:uid="{07879B7E-CD05-3645-9E0D-C02E457F8A30}">
       <formula1>"Day"</formula1>
@@ -1066,11 +1064,11 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Required variable names cannot be adjusted" promptTitle="SD of Membrane Diameter" prompt="mm" sqref="M1" xr:uid="{5E062560-D995-ED43-B31B-3714167866DF}">
       <formula1>"Membrane_SD"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Required variable names cannot be adjusted" promptTitle="Average Yolk Diameter" prompt="mm" sqref="N1" xr:uid="{34E4634C-9163-DD43-9E5A-2D39B0C85040}">
-      <formula1>"Yolk_Ave"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Required variable names cannot be adjusted" promptTitle="SD of Yolk Diameter" prompt="mm" sqref="O1" xr:uid="{0648FFCD-3D8F-AE42-A443-E270DBE8FDF5}">
-      <formula1>"Yolk_SD"</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Required variable names cannot be adjusted" promptTitle="Average Embryo Diameter" prompt="mm" sqref="N1" xr:uid="{34E4634C-9163-DD43-9E5A-2D39B0C85040}">
+      <formula1>"Embryo_Ave"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Required variable names cannot be adjusted" promptTitle="SD of Embryo Diameter" prompt="mm" sqref="O1" xr:uid="{0648FFCD-3D8F-AE42-A443-E270DBE8FDF5}">
+      <formula1>"Embryo_SD"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Required variable names cannot be adjusted" promptTitle="Midline Larval Length" prompt="mm" sqref="P1" xr:uid="{46DABF2E-5904-0F42-A7AB-178D4B1F828B}">
       <formula1>"Larval_Length"</formula1>

</xml_diff>